<commit_message>
Michal Monselise withdrew from team, is working alone.
</commit_message>
<xml_diff>
--- a/UWKT3_TeamRoster.xlsx
+++ b/UWKT3_TeamRoster.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="143">
   <si>
     <t>Full</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>gphogue@gmail.com</t>
+  </si>
+  <si>
+    <t>wernercolangelo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1141,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1146,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1194,67 +1197,41 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H5" t="s">
-        <v>133</v>
-      </c>
-    </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>117</v>
-      </c>
       <c r="G6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
         <v>3</v>
@@ -1263,76 +1240,76 @@
         <v>117</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>141</v>
+        <v>120</v>
+      </c>
+      <c r="H7" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2">
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
-      </c>
-      <c r="H8" t="s">
-        <v>135</v>
+        <v>121</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="G9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E10" s="2">
         <v>3</v>
@@ -1341,24 +1318,24 @@
         <v>117</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2">
         <v>3</v>
@@ -1367,24 +1344,24 @@
         <v>117</v>
       </c>
       <c r="G11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
         <v>3</v>
@@ -1393,46 +1370,86 @@
         <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="E13" s="2">
         <v>3</v>
       </c>
       <c r="F13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
         <v>128</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>127</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="D15" t="s">
+    <row r="16" spans="1:8">
+      <c r="D16" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1"/>
+    <hyperlink ref="H8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Werner Colangelo is not part of Team 3.
</commit_message>
<xml_diff>
--- a/UWKT3_TeamRoster.xlsx
+++ b/UWKT3_TeamRoster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31520" yWindow="14300" windowWidth="13840" windowHeight="13940"/>
+    <workbookView xWindow="32540" yWindow="14180" windowWidth="13840" windowHeight="13940"/>
   </bookViews>
   <sheets>
     <sheet name="UWKT3" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="143">
   <si>
     <t>Full</t>
   </si>
@@ -448,7 +448,7 @@
     <t>gphogue@gmail.com</t>
   </si>
   <si>
-    <t>wernercolangelo@gmail.com</t>
+    <t>Chose to work alone.</t>
   </si>
 </sst>
 </file>
@@ -480,7 +480,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +490,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,11 +683,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="171"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="172">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1149,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1161,17 +1168,17 @@
     <col min="8" max="8" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1204,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1227,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1246,7 +1253,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -1272,7 +1279,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>80</v>
       </c>
@@ -1298,33 +1305,36 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -1350,7 +1360,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>88</v>
       </c>
@@ -1402,7 +1412,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -1428,23 +1438,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="D16" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Helper script for munging Weka ARFF classifier output in csv submittal file.
</commit_message>
<xml_diff>
--- a/UWKT3_TeamRoster.xlsx
+++ b/UWKT3_TeamRoster.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32540" yWindow="14180" windowWidth="13840" windowHeight="13940"/>
+    <workbookView xWindow="27600" yWindow="9360" windowWidth="13840" windowHeight="13940"/>
   </bookViews>
   <sheets>
     <sheet name="UWKT3" sheetId="2" r:id="rId1"/>
     <sheet name="AllTeams" sheetId="1" r:id="rId2"/>
+    <sheet name="Submissions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="147">
   <si>
     <t>Full</t>
   </si>
@@ -424,9 +425,6 @@
     <t>betbritt@u.washington.edu</t>
   </si>
   <si>
-    <t>ewingam@uw.edu</t>
-  </si>
-  <si>
     <t>pat@patleahy.com</t>
   </si>
   <si>
@@ -449,6 +447,21 @@
   </si>
   <si>
     <t>Chose to work alone.</t>
+  </si>
+  <si>
+    <t>Submissions</t>
+  </si>
+  <si>
+    <t>ewing.andy@gmail.com</t>
+  </si>
+  <si>
+    <t>See UWKT3_Submissions.xlsx</t>
+  </si>
+  <si>
+    <t>Submittal?</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -509,7 +522,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="172">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -682,6 +695,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -690,7 +706,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="171"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="172">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -776,6 +792,9 @@
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1156,296 +1175,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="8" max="8" width="24.5" customWidth="1"/>
+    <col min="1" max="2" width="15" customWidth="1"/>
+    <col min="9" max="9" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>115</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>116</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>118</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>119</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>117</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>120</v>
       </c>
-      <c r="H7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>117</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>121</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>128</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>122</v>
       </c>
-      <c r="H9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>3</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="I10" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>135</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>117</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>124</v>
       </c>
-      <c r="H11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>117</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>125</v>
       </c>
-      <c r="H12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>117</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>126</v>
       </c>
-      <c r="H13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="I13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>128</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>127</v>
       </c>
-      <c r="H14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="D16" t="s">
+      <c r="I14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="E16" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
+    <hyperlink ref="I8" r:id="rId1"/>
+    <hyperlink ref="I7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2040,4 +2082,37 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="4" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Submissions updated to reflect Andy Ewings 0.71862 submission. Snapshot before substantially revising report to send out to team for review and additions.
</commit_message>
<xml_diff>
--- a/UWKT3_TeamRoster.xlsx
+++ b/UWKT3_TeamRoster.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27600" yWindow="9360" windowWidth="13840" windowHeight="13940"/>
+    <workbookView xWindow="7760" yWindow="12520" windowWidth="13840" windowHeight="13940"/>
   </bookViews>
   <sheets>
     <sheet name="UWKT3" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="147">
   <si>
     <t>Full</t>
   </si>
@@ -1167,7 +1167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1254,7 +1254,9 @@
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>